<commit_message>
Starting to transfer to splitting by number of shipments
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\UniZeug\AbfallGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A980E8B6-FE61-4767-B791-B36A3998497B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85719A83-0425-4535-A2E7-747DF0314CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview2" sheetId="7" r:id="rId1"/>
@@ -784,6 +784,1459 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>JSprit</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Computation Time in Relation to Number of Shipments</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11563888888888889"/>
+          <c:y val="1.3888888888888888E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12630314960629924"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.83247462817147855"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SizeTime</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Carriers_stats-geo2'!$G$2:$G$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Carriers_stats-geo2'!$R$2:$R$61</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1574074074074073E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3148148148148147E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6296296296296294E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7870370370370373E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6296296296296294E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1018518518518516E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.9444444444444444E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.273148148148148E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7870370370370373E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7361111111111112E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5462962962962961E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3888888888888889E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7037037037037035E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3981481481481481E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.4398148148148144E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7361111111111112E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.2824074074074075E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.7453703703703704E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4305555555555555E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.3657407407407413E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.9861111111111116E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.134259259259259E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.2500000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.7870370370370367E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.2962962962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.1435185185185185E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4699074074074074E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.6087962962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.7129629629629625E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.7592592592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.7939814814814815E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.2152777777777778E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.724537037037037E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.6435185185185185E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4583333333333334E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.9675925925925924E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4236111111111112E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.0486111111111113E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.1458333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.685185185185185E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.2337962962962962E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.3148148148148147E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.4189814814814816E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.31712962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.8587962962962963E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.0810185185185186E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.4629629629629629E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.7453703703703703E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.9675925925925929E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.3796296296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.8958333333333329E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.4861111111111109E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.5787037037037038E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.7361111111111112E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.375E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C5F7-4FF9-93A1-DFFFE48D387B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="555479944"/>
+        <c:axId val="555478144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="555479944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Shipments</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555478144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="555478144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>JSprit</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Computation Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.6319626713327489E-3"/>
+              <c:y val="0.36106964890258281"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555479944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{903A2B98-5C7B-9945-C412-6B9D334FEEB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_5" connectionId="3" xr16:uid="{C298B43C-66F9-49FE-8067-D43A20E6C362}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="19">
@@ -976,6 +2429,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C452F4A1-573B-4604-AAC0-9C16505809FA}" name="Carriers_stats" displayName="Carriers_stats" ref="A1:R61" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:R61" xr:uid="{C452F4A1-573B-4604-AAC0-9C16505809FA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R61">
+    <sortCondition ref="G1:G61"/>
+  </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{86EEA6CE-6255-4F8E-A647-97A8AE20AF40}" uniqueName="1" name="carrierId" queryTableFieldId="1" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{54D92DC2-6CE5-4706-9AF6-4A68750AF1F4}" uniqueName="2" name="nuOfJspritIterations" queryTableFieldId="2"/>
@@ -1335,7 +2791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85273B5F-83F8-4430-AB26-19A70B48FB20}">
   <dimension ref="B2:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1442,11 +2898,11 @@
       </c>
       <c r="C5" s="12">
         <f>'Carriers_stats-geo2'!J62</f>
-        <v>-192294.19944953761</v>
+        <v>-192294.19944953758</v>
       </c>
       <c r="D5" s="14">
         <f>C5/C3 -1</f>
-        <v>8.7094231549099232E-2</v>
+        <v>8.709423154909901E-2</v>
       </c>
       <c r="E5" s="12">
         <f>'Carriers_stats-geo2'!K62</f>
@@ -1458,7 +2914,7 @@
       </c>
       <c r="G5" s="13">
         <f>'Carriers_stats-geo2'!R62</f>
-        <v>0.12480324074074076</v>
+        <v>0.12480324074074074</v>
       </c>
       <c r="H5" s="14">
         <f>G5/G3 -1</f>
@@ -6198,8 +7654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6392B58-0D3B-4607-B2BA-B7B85C8C2B37}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="I27" workbookViewId="0">
-      <selection activeCell="R63" sqref="R63"/>
+    <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6280,7 +7736,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -6298,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -6307,36 +7763,36 @@
         <v>20</v>
       </c>
       <c r="J2">
-        <v>-1862.1873215870501</v>
+        <v>-926.05786816995408</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
       <c r="M2">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="N2">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>24991</v>
+        <v>13652</v>
       </c>
       <c r="Q2">
-        <v>24991</v>
+        <v>13652</v>
       </c>
       <c r="R2" s="1">
-        <v>5.7870370370370373E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -6354,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -6363,36 +7819,36 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <v>-1863.5627669883063</v>
+        <v>-876.7772747587469</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
         <v>21</v>
       </c>
       <c r="M3">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="N3">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>28534</v>
+        <v>11125</v>
       </c>
       <c r="Q3">
-        <v>28534</v>
+        <v>11125</v>
       </c>
       <c r="R3" s="1">
-        <v>8.1018518518518516E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -6410,7 +7866,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -6419,36 +7875,36 @@
         <v>20</v>
       </c>
       <c r="J4">
-        <v>-1898.4368283901219</v>
+        <v>-875.6435462802142</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>21</v>
       </c>
       <c r="M4">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="N4">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>26745</v>
+        <v>11183</v>
       </c>
       <c r="Q4">
-        <v>26745</v>
+        <v>11183</v>
       </c>
       <c r="R4" s="1">
-        <v>4.6296296296296294E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -6466,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>498</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -6475,36 +7931,36 @@
         <v>20</v>
       </c>
       <c r="J5">
-        <v>-11341.325407331695</v>
+        <v>-931.51751441542706</v>
       </c>
       <c r="K5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
         <v>21</v>
       </c>
       <c r="M5">
-        <v>498</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>498</v>
+        <v>25</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>166216</v>
+        <v>13566</v>
       </c>
       <c r="Q5">
-        <v>166216</v>
+        <v>13566</v>
       </c>
       <c r="R5" s="1">
-        <v>5.5787037037037038E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -6522,7 +7978,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>261</v>
+        <v>32</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -6531,36 +7987,36 @@
         <v>20</v>
       </c>
       <c r="J6">
-        <v>-5753.891909735994</v>
+        <v>-895.19877371432551</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
         <v>21</v>
       </c>
       <c r="M6">
-        <v>261</v>
+        <v>32</v>
       </c>
       <c r="N6">
-        <v>261</v>
+        <v>32</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>87255</v>
+        <v>14612</v>
       </c>
       <c r="Q6">
-        <v>87255</v>
+        <v>14612</v>
       </c>
       <c r="R6" s="1">
-        <v>1.1458333333333333E-3</v>
+        <v>1.1574074074074073E-5</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -6578,7 +8034,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>251</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -6587,36 +8043,36 @@
         <v>20</v>
       </c>
       <c r="J7">
-        <v>-4771.8203074020012</v>
+        <v>-893.23180561521679</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L7" t="s">
         <v>21</v>
       </c>
       <c r="M7">
-        <v>251</v>
+        <v>39</v>
       </c>
       <c r="N7">
-        <v>251</v>
+        <v>39</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>64669</v>
+        <v>6868</v>
       </c>
       <c r="Q7">
-        <v>64669</v>
+        <v>6868</v>
       </c>
       <c r="R7" s="1">
-        <v>1.4236111111111112E-3</v>
+        <v>2.3148148148148147E-5</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -6634,7 +8090,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>233</v>
+        <v>51</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -6643,36 +8099,36 @@
         <v>20</v>
       </c>
       <c r="J8">
-        <v>-3515.6777504546549</v>
+        <v>-925.77185262193802</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
         <v>21</v>
       </c>
       <c r="M8">
-        <v>233</v>
+        <v>51</v>
       </c>
       <c r="N8">
-        <v>233</v>
+        <v>51</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>64711</v>
+        <v>22661</v>
       </c>
       <c r="Q8">
-        <v>64711</v>
+        <v>22661</v>
       </c>
       <c r="R8" s="1">
-        <v>1.6435185185185185E-3</v>
+        <v>4.6296296296296294E-5</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -6690,7 +8146,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>210</v>
+        <v>57</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -6699,36 +8155,36 @@
         <v>20</v>
       </c>
       <c r="J9">
-        <v>-2702.5536388207065</v>
+        <v>-1862.1873215870501</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
         <v>21</v>
       </c>
       <c r="M9">
-        <v>210</v>
+        <v>57</v>
       </c>
       <c r="N9">
-        <v>210</v>
+        <v>57</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>65235</v>
+        <v>24991</v>
       </c>
       <c r="Q9">
-        <v>65235</v>
+        <v>24991</v>
       </c>
       <c r="R9" s="1">
-        <v>1.2152777777777778E-3</v>
+        <v>5.7870370370370373E-5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -6746,7 +8202,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -6755,7 +8211,7 @@
         <v>20</v>
       </c>
       <c r="J10">
-        <v>-1778.7556858230791</v>
+        <v>-1898.4368283901219</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -6764,27 +8220,27 @@
         <v>21</v>
       </c>
       <c r="M10">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="N10">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>39954</v>
+        <v>26745</v>
       </c>
       <c r="Q10">
-        <v>39954</v>
+        <v>26745</v>
       </c>
       <c r="R10" s="1">
-        <v>4.2824074074074075E-4</v>
+        <v>4.6296296296296294E-5</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -6802,7 +8258,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -6811,36 +8267,36 @@
         <v>20</v>
       </c>
       <c r="J11">
-        <v>-875.6435462802142</v>
+        <v>-1863.5627669883063</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" t="s">
         <v>21</v>
       </c>
       <c r="M11">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="N11">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
-        <v>11183</v>
+        <v>28534</v>
       </c>
       <c r="Q11">
-        <v>11183</v>
+        <v>28534</v>
       </c>
       <c r="R11" s="1">
-        <v>0</v>
+        <v>8.1018518518518516E-5</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -6858,7 +8314,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -6867,36 +8323,36 @@
         <v>20</v>
       </c>
       <c r="J12">
-        <v>-876.7772747587469</v>
+        <v>-1853.2484061487128</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" t="s">
         <v>21</v>
       </c>
       <c r="M12">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="N12">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>11125</v>
+        <v>34887</v>
       </c>
       <c r="Q12">
-        <v>11125</v>
+        <v>34887</v>
       </c>
       <c r="R12" s="1">
-        <v>0</v>
+        <v>6.9444444444444444E-5</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -6914,7 +8370,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -6923,36 +8379,36 @@
         <v>20</v>
       </c>
       <c r="J13">
-        <v>-895.19877371432551</v>
+        <v>-1868.1016272146335</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" t="s">
         <v>21</v>
       </c>
       <c r="M13">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="N13">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13">
-        <v>14612</v>
+        <v>19955</v>
       </c>
       <c r="Q13">
-        <v>14612</v>
+        <v>19955</v>
       </c>
       <c r="R13" s="1">
-        <v>1.1574074074074073E-5</v>
+        <v>1.273148148148148E-4</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -6970,7 +8426,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -6979,36 +8435,36 @@
         <v>20</v>
       </c>
       <c r="J14">
-        <v>-906.2132483311841</v>
+        <v>-2779.4703598450242</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L14" t="s">
         <v>21</v>
       </c>
       <c r="M14">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="N14">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14">
-        <v>10386</v>
+        <v>42853</v>
       </c>
       <c r="Q14">
-        <v>10386</v>
+        <v>42853</v>
       </c>
       <c r="R14" s="1">
-        <v>4.3981481481481481E-4</v>
+        <v>5.7870370370370373E-5</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -7026,7 +8482,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -7035,7 +8491,7 @@
         <v>20</v>
       </c>
       <c r="J15">
-        <v>-893.23180561521679</v>
+        <v>-911.22656639553634</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -7044,27 +8500,27 @@
         <v>21</v>
       </c>
       <c r="M15">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="N15">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
-        <v>6868</v>
+        <v>18196</v>
       </c>
       <c r="Q15">
-        <v>6868</v>
+        <v>18196</v>
       </c>
       <c r="R15" s="1">
-        <v>2.3148148148148147E-5</v>
+        <v>1.7361111111111112E-4</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -7082,7 +8538,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -7091,36 +8547,36 @@
         <v>20</v>
       </c>
       <c r="J16">
-        <v>-1807.9104498208733</v>
+        <v>-919.19021381044945</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" t="s">
         <v>21</v>
       </c>
       <c r="M16">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="N16">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16">
-        <v>20096</v>
+        <v>13792</v>
       </c>
       <c r="Q16">
-        <v>20096</v>
+        <v>13792</v>
       </c>
       <c r="R16" s="1">
-        <v>7.9861111111111116E-4</v>
+        <v>2.5462962962962961E-4</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -7138,7 +8594,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>347</v>
+        <v>87</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -7147,36 +8603,36 @@
         <v>20</v>
       </c>
       <c r="J17">
-        <v>-8341.8231502604522</v>
+        <v>-1845.0534937857976</v>
       </c>
       <c r="K17">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L17" t="s">
         <v>21</v>
       </c>
       <c r="M17">
-        <v>347</v>
+        <v>87</v>
       </c>
       <c r="N17">
-        <v>347</v>
+        <v>87</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17">
-        <v>105397</v>
+        <v>31718</v>
       </c>
       <c r="Q17">
-        <v>105397</v>
+        <v>31718</v>
       </c>
       <c r="R17" s="1">
-        <v>2.8587962962962963E-3</v>
+        <v>1.3888888888888889E-4</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18">
         <v>100</v>
@@ -7194,7 +8650,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -7203,36 +8659,36 @@
         <v>20</v>
       </c>
       <c r="J18">
-        <v>-3821.0209713652116</v>
+        <v>-965.31635765686917</v>
       </c>
       <c r="K18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L18" t="s">
         <v>21</v>
       </c>
       <c r="M18">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="N18">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18">
-        <v>54050</v>
+        <v>12565</v>
       </c>
       <c r="Q18">
-        <v>54050</v>
+        <v>12565</v>
       </c>
       <c r="R18" s="1">
-        <v>6.7129629629629625E-4</v>
+        <v>3.7037037037037035E-4</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -7250,7 +8706,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -7259,36 +8715,36 @@
         <v>20</v>
       </c>
       <c r="J19">
-        <v>-2815.455327720837</v>
+        <v>-906.2132483311841</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L19" t="s">
         <v>21</v>
       </c>
       <c r="M19">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="N19">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19">
-        <v>34483</v>
+        <v>10386</v>
       </c>
       <c r="Q19">
-        <v>34483</v>
+        <v>10386</v>
       </c>
       <c r="R19" s="1">
-        <v>1.7361111111111112E-4</v>
+        <v>4.3981481481481481E-4</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>100</v>
@@ -7306,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -7315,36 +8771,36 @@
         <v>20</v>
       </c>
       <c r="J20">
-        <v>-1889.6461097065567</v>
+        <v>-919.89211762424827</v>
       </c>
       <c r="K20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" t="s">
         <v>21</v>
       </c>
       <c r="M20">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="N20">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20">
-        <v>26552</v>
+        <v>15838</v>
       </c>
       <c r="Q20">
-        <v>26552</v>
+        <v>15838</v>
       </c>
       <c r="R20" s="1">
-        <v>1.6087962962962963E-3</v>
+        <v>5.4398148148148144E-4</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -7362,7 +8818,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -7371,36 +8827,36 @@
         <v>20</v>
       </c>
       <c r="J21">
-        <v>-965.31635765686917</v>
+        <v>-2815.455327720837</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L21" t="s">
         <v>21</v>
       </c>
       <c r="M21">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N21">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
-        <v>12565</v>
+        <v>34483</v>
       </c>
       <c r="Q21">
-        <v>12565</v>
+        <v>34483</v>
       </c>
       <c r="R21" s="1">
-        <v>3.7037037037037035E-4</v>
+        <v>1.7361111111111112E-4</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -7418,7 +8874,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -7427,36 +8883,36 @@
         <v>20</v>
       </c>
       <c r="J22">
-        <v>-2765.4643755194797</v>
+        <v>-1778.7556858230791</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L22" t="s">
         <v>21</v>
       </c>
       <c r="M22">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="N22">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
-        <v>25923</v>
+        <v>39954</v>
       </c>
       <c r="Q22">
-        <v>25923</v>
+        <v>39954</v>
       </c>
       <c r="R22" s="1">
-        <v>1.7592592592592592E-3</v>
+        <v>4.2824074074074075E-4</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -7474,7 +8930,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -7483,36 +8939,36 @@
         <v>20</v>
       </c>
       <c r="J23">
-        <v>-2858.5602368962286</v>
+        <v>-1812.5761087554479</v>
       </c>
       <c r="K23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L23" t="s">
         <v>21</v>
       </c>
       <c r="M23">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="N23">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>38144</v>
+        <v>33303</v>
       </c>
       <c r="Q23">
-        <v>38144</v>
+        <v>33303</v>
       </c>
       <c r="R23" s="1">
-        <v>5.7870370370370367E-4</v>
+        <v>4.7453703703703704E-4</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -7530,7 +8986,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -7539,36 +8995,36 @@
         <v>20</v>
       </c>
       <c r="J24">
-        <v>-1868.1016272146335</v>
+        <v>-3675.480661697949</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L24" t="s">
         <v>21</v>
       </c>
       <c r="M24">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="N24">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24">
-        <v>19955</v>
+        <v>59859</v>
       </c>
       <c r="Q24">
-        <v>19955</v>
+        <v>59859</v>
       </c>
       <c r="R24" s="1">
-        <v>1.273148148148148E-4</v>
+        <v>2.4305555555555555E-4</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -7586,7 +9042,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -7595,36 +9051,36 @@
         <v>20</v>
       </c>
       <c r="J25">
-        <v>-2855.895103173641</v>
+        <v>-1812.0397117984292</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L25" t="s">
         <v>21</v>
       </c>
       <c r="M25">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="N25">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
       <c r="P25">
-        <v>39161</v>
+        <v>25192</v>
       </c>
       <c r="Q25">
-        <v>39161</v>
+        <v>25192</v>
       </c>
       <c r="R25" s="1">
-        <v>6.2500000000000001E-4</v>
+        <v>6.3657407407407413E-4</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B26">
         <v>100</v>
@@ -7642,7 +9098,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -7651,36 +9107,36 @@
         <v>20</v>
       </c>
       <c r="J26">
-        <v>-926.05786816995408</v>
+        <v>-1807.9104498208733</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L26" t="s">
         <v>21</v>
       </c>
       <c r="M26">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="N26">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <v>13652</v>
+        <v>20096</v>
       </c>
       <c r="Q26">
-        <v>13652</v>
+        <v>20096</v>
       </c>
       <c r="R26" s="1">
-        <v>0</v>
+        <v>7.9861111111111116E-4</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B27">
         <v>100</v>
@@ -7698,7 +9154,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -7707,36 +9163,36 @@
         <v>20</v>
       </c>
       <c r="J27">
-        <v>-1853.2484061487128</v>
+        <v>-2658.3945948175742</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L27" t="s">
         <v>21</v>
       </c>
       <c r="M27">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="N27">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27">
-        <v>34887</v>
+        <v>35759</v>
       </c>
       <c r="Q27">
-        <v>34887</v>
+        <v>35759</v>
       </c>
       <c r="R27" s="1">
-        <v>6.9444444444444444E-5</v>
+        <v>6.134259259259259E-4</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28">
         <v>100</v>
@@ -7754,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -7763,36 +9219,36 @@
         <v>20</v>
       </c>
       <c r="J28">
-        <v>-925.77185262193802</v>
+        <v>-2855.895103173641</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L28" t="s">
         <v>21</v>
       </c>
       <c r="M28">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="N28">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
       <c r="P28">
-        <v>22661</v>
+        <v>39161</v>
       </c>
       <c r="Q28">
-        <v>22661</v>
+        <v>39161</v>
       </c>
       <c r="R28" s="1">
-        <v>4.6296296296296294E-5</v>
+        <v>6.2500000000000001E-4</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>100</v>
@@ -7810,7 +9266,7 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>238</v>
+        <v>161</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -7819,7 +9275,7 @@
         <v>20</v>
       </c>
       <c r="J29">
-        <v>-2760.2768406375326</v>
+        <v>-2858.5602368962286</v>
       </c>
       <c r="K29">
         <v>3</v>
@@ -7828,27 +9284,27 @@
         <v>21</v>
       </c>
       <c r="M29">
-        <v>238</v>
+        <v>161</v>
       </c>
       <c r="N29">
-        <v>238</v>
+        <v>161</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="P29">
-        <v>62446</v>
+        <v>38144</v>
       </c>
       <c r="Q29">
-        <v>62446</v>
+        <v>38144</v>
       </c>
       <c r="R29" s="1">
-        <v>1.9675925925925924E-3</v>
+        <v>5.7870370370370367E-4</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>100</v>
@@ -7866,7 +9322,7 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>361</v>
+        <v>161</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -7875,36 +9331,36 @@
         <v>20</v>
       </c>
       <c r="J30">
-        <v>-3676.7369592406326</v>
+        <v>-1806.2484831788984</v>
       </c>
       <c r="K30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L30" t="s">
         <v>21</v>
       </c>
       <c r="M30">
-        <v>361</v>
+        <v>161</v>
       </c>
       <c r="N30">
-        <v>361</v>
+        <v>161</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
-        <v>91105</v>
+        <v>22910</v>
       </c>
       <c r="Q30">
-        <v>91105</v>
+        <v>22910</v>
       </c>
       <c r="R30" s="1">
-        <v>4.7453703703703703E-3</v>
+        <v>1.2962962962962963E-3</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B31">
         <v>100</v>
@@ -7922,7 +9378,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -7931,36 +9387,36 @@
         <v>20</v>
       </c>
       <c r="J31">
-        <v>-2658.3945948175742</v>
+        <v>-1875.6391554812008</v>
       </c>
       <c r="K31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L31" t="s">
         <v>21</v>
       </c>
       <c r="M31">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="N31">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>35759</v>
+        <v>28405</v>
       </c>
       <c r="Q31">
-        <v>35759</v>
+        <v>28405</v>
       </c>
       <c r="R31" s="1">
-        <v>6.134259259259259E-4</v>
+        <v>9.1435185185185185E-4</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B32">
         <v>100</v>
@@ -7978,7 +9434,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -7987,7 +9443,7 @@
         <v>20</v>
       </c>
       <c r="J32">
-        <v>-1845.0534937857976</v>
+        <v>-1803.7021737658026</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -7996,27 +9452,27 @@
         <v>21</v>
       </c>
       <c r="M32">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="N32">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="P32">
-        <v>31718</v>
+        <v>28887</v>
       </c>
       <c r="Q32">
-        <v>31718</v>
+        <v>28887</v>
       </c>
       <c r="R32" s="1">
-        <v>1.3888888888888889E-4</v>
+        <v>1.4699074074074074E-3</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B33">
         <v>100</v>
@@ -8034,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -8043,36 +9499,36 @@
         <v>20</v>
       </c>
       <c r="J33">
-        <v>-2779.4703598450242</v>
+        <v>-1870.610005459376</v>
       </c>
       <c r="K33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L33" t="s">
         <v>21</v>
       </c>
       <c r="M33">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="N33">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="P33">
-        <v>42853</v>
+        <v>42531</v>
       </c>
       <c r="Q33">
-        <v>42853</v>
+        <v>42531</v>
       </c>
       <c r="R33" s="1">
-        <v>5.7870370370370373E-5</v>
+        <v>1.1111111111111111E-3</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B34">
         <v>100</v>
@@ -8090,7 +9546,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -8099,36 +9555,36 @@
         <v>20</v>
       </c>
       <c r="J34">
-        <v>-3675.480661697949</v>
+        <v>-1889.6461097065567</v>
       </c>
       <c r="K34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L34" t="s">
         <v>21</v>
       </c>
       <c r="M34">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="N34">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
-        <v>59859</v>
+        <v>26552</v>
       </c>
       <c r="Q34">
-        <v>59859</v>
+        <v>26552</v>
       </c>
       <c r="R34" s="1">
-        <v>2.4305555555555555E-4</v>
+        <v>1.6087962962962963E-3</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -8146,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>404</v>
+        <v>190</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -8155,36 +9611,36 @@
         <v>20</v>
       </c>
       <c r="J35">
-        <v>-9236.5008999071706</v>
+        <v>-3821.0209713652116</v>
       </c>
       <c r="K35">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L35" t="s">
         <v>21</v>
       </c>
       <c r="M35">
-        <v>404</v>
+        <v>190</v>
       </c>
       <c r="N35">
-        <v>404</v>
+        <v>190</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
       <c r="P35">
-        <v>139711</v>
+        <v>54050</v>
       </c>
       <c r="Q35">
-        <v>139711</v>
+        <v>54050</v>
       </c>
       <c r="R35" s="1">
-        <v>3.3796296296296296E-3</v>
+        <v>6.7129629629629625E-4</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -8202,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>309</v>
+        <v>204</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -8211,36 +9667,36 @@
         <v>20</v>
       </c>
       <c r="J36">
-        <v>-6497.6808058318993</v>
+        <v>-2765.4643755194797</v>
       </c>
       <c r="K36">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L36" t="s">
         <v>21</v>
       </c>
       <c r="M36">
-        <v>309</v>
+        <v>204</v>
       </c>
       <c r="N36">
-        <v>309</v>
+        <v>204</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
       <c r="P36">
-        <v>99763</v>
+        <v>25923</v>
       </c>
       <c r="Q36">
-        <v>99763</v>
+        <v>25923</v>
       </c>
       <c r="R36" s="1">
-        <v>2.4189814814814816E-3</v>
+        <v>1.7592592592592592E-3</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B37">
         <v>100</v>
@@ -8258,7 +9714,7 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <v>489</v>
+        <v>205</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -8267,36 +9723,36 @@
         <v>20</v>
       </c>
       <c r="J37">
-        <v>-9333.8475253964734</v>
+        <v>-1877.7194518025144</v>
       </c>
       <c r="K37">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L37" t="s">
         <v>21</v>
       </c>
       <c r="M37">
-        <v>489</v>
+        <v>205</v>
       </c>
       <c r="N37">
-        <v>489</v>
+        <v>205</v>
       </c>
       <c r="O37">
         <v>0</v>
       </c>
       <c r="P37">
-        <v>157856</v>
+        <v>34921</v>
       </c>
       <c r="Q37">
-        <v>157856</v>
+        <v>34921</v>
       </c>
       <c r="R37" s="1">
-        <v>5.4861111111111109E-3</v>
+        <v>1.7939814814814815E-3</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B38">
         <v>100</v>
@@ -8314,7 +9770,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -8323,31 +9779,31 @@
         <v>20</v>
       </c>
       <c r="J38">
-        <v>-1812.5761087554479</v>
+        <v>-2702.5536388207065</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L38" t="s">
         <v>21</v>
       </c>
       <c r="M38">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="N38">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="O38">
         <v>0</v>
       </c>
       <c r="P38">
-        <v>33303</v>
+        <v>65235</v>
       </c>
       <c r="Q38">
-        <v>33303</v>
+        <v>65235</v>
       </c>
       <c r="R38" s="1">
-        <v>4.7453703703703704E-4</v>
+        <v>1.2152777777777778E-3</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -8408,7 +9864,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="B40">
         <v>100</v>
@@ -8426,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -8435,7 +9891,7 @@
         <v>20</v>
       </c>
       <c r="J40">
-        <v>-3712.4643920532985</v>
+        <v>-3515.6777504546549</v>
       </c>
       <c r="K40">
         <v>4</v>
@@ -8444,27 +9900,27 @@
         <v>21</v>
       </c>
       <c r="M40">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="N40">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="O40">
         <v>0</v>
       </c>
       <c r="P40">
-        <v>68056</v>
+        <v>64711</v>
       </c>
       <c r="Q40">
-        <v>68056</v>
+        <v>64711</v>
       </c>
       <c r="R40" s="1">
-        <v>2.685185185185185E-3</v>
+        <v>1.6435185185185185E-3</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B41">
         <v>100</v>
@@ -8482,7 +9938,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>84</v>
+        <v>234</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -8491,36 +9947,36 @@
         <v>20</v>
       </c>
       <c r="J41">
-        <v>-919.19021381044945</v>
+        <v>-2797.8341937105984</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L41" t="s">
         <v>21</v>
       </c>
       <c r="M41">
-        <v>84</v>
+        <v>234</v>
       </c>
       <c r="N41">
-        <v>84</v>
+        <v>234</v>
       </c>
       <c r="O41">
         <v>0</v>
       </c>
       <c r="P41">
-        <v>13792</v>
+        <v>46134</v>
       </c>
       <c r="Q41">
-        <v>13792</v>
+        <v>46134</v>
       </c>
       <c r="R41" s="1">
-        <v>2.5462962962962961E-4</v>
+        <v>1.4583333333333334E-3</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B42">
         <v>100</v>
@@ -8538,7 +9994,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -8547,36 +10003,36 @@
         <v>20</v>
       </c>
       <c r="J42">
-        <v>-919.89211762424827</v>
+        <v>-2760.2768406375326</v>
       </c>
       <c r="K42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L42" t="s">
         <v>21</v>
       </c>
       <c r="M42">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="N42">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="O42">
         <v>0</v>
       </c>
       <c r="P42">
-        <v>15838</v>
+        <v>62446</v>
       </c>
       <c r="Q42">
-        <v>15838</v>
+        <v>62446</v>
       </c>
       <c r="R42" s="1">
-        <v>5.4398148148148144E-4</v>
+        <v>1.9675925925925924E-3</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>100</v>
@@ -8594,7 +10050,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -8603,36 +10059,36 @@
         <v>20</v>
       </c>
       <c r="J43">
-        <v>-1806.2484831788984</v>
+        <v>-4771.8203074020012</v>
       </c>
       <c r="K43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L43" t="s">
         <v>21</v>
       </c>
       <c r="M43">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="N43">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="O43">
         <v>0</v>
       </c>
       <c r="P43">
-        <v>22910</v>
+        <v>64669</v>
       </c>
       <c r="Q43">
-        <v>22910</v>
+        <v>64669</v>
       </c>
       <c r="R43" s="1">
-        <v>1.2962962962962963E-3</v>
+        <v>1.4236111111111112E-3</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B44">
         <v>100</v>
@@ -8650,7 +10106,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>340</v>
+        <v>251</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -8659,36 +10115,36 @@
         <v>20</v>
       </c>
       <c r="J44">
-        <v>-4598.7146838560748</v>
+        <v>-3578.8318897373438</v>
       </c>
       <c r="K44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L44" t="s">
         <v>21</v>
       </c>
       <c r="M44">
-        <v>340</v>
+        <v>251</v>
       </c>
       <c r="N44">
-        <v>340</v>
+        <v>251</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
       <c r="P44">
-        <v>70524</v>
+        <v>54241</v>
       </c>
       <c r="Q44">
-        <v>70524</v>
+        <v>54241</v>
       </c>
       <c r="R44" s="1">
-        <v>4.31712962962963E-3</v>
+        <v>2.0486111111111113E-3</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>100</v>
@@ -8706,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <v>305</v>
+        <v>261</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -8715,7 +10171,7 @@
         <v>20</v>
       </c>
       <c r="J45">
-        <v>-5601.3752998833024</v>
+        <v>-5753.891909735994</v>
       </c>
       <c r="K45">
         <v>6</v>
@@ -8724,27 +10180,27 @@
         <v>21</v>
       </c>
       <c r="M45">
-        <v>305</v>
+        <v>261</v>
       </c>
       <c r="N45">
-        <v>305</v>
+        <v>261</v>
       </c>
       <c r="O45">
         <v>0</v>
       </c>
       <c r="P45">
-        <v>85524</v>
+        <v>87255</v>
       </c>
       <c r="Q45">
-        <v>85524</v>
+        <v>87255</v>
       </c>
       <c r="R45" s="1">
-        <v>2.3148148148148147E-3</v>
+        <v>1.1458333333333333E-3</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B46">
         <v>100</v>
@@ -8762,7 +10218,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>616</v>
+        <v>285</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -8771,36 +10227,36 @@
         <v>20</v>
       </c>
       <c r="J46">
-        <v>-8329.2999785437587</v>
+        <v>-3712.4643920532985</v>
       </c>
       <c r="K46">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L46" t="s">
         <v>21</v>
       </c>
       <c r="M46">
-        <v>616</v>
+        <v>285</v>
       </c>
       <c r="N46">
-        <v>616</v>
+        <v>285</v>
       </c>
       <c r="O46">
         <v>0</v>
       </c>
       <c r="P46">
-        <v>137832</v>
+        <v>68056</v>
       </c>
       <c r="Q46">
-        <v>137832</v>
+        <v>68056</v>
       </c>
       <c r="R46" s="1">
-        <v>1.375E-2</v>
+        <v>2.685185185185185E-3</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B47">
         <v>100</v>
@@ -8818,7 +10274,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>234</v>
+        <v>296</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -8827,36 +10283,36 @@
         <v>20</v>
       </c>
       <c r="J47">
-        <v>-2797.8341937105984</v>
+        <v>-4619.0395607109003</v>
       </c>
       <c r="K47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L47" t="s">
         <v>21</v>
       </c>
       <c r="M47">
-        <v>234</v>
+        <v>296</v>
       </c>
       <c r="N47">
-        <v>234</v>
+        <v>296</v>
       </c>
       <c r="O47">
         <v>0</v>
       </c>
       <c r="P47">
-        <v>46134</v>
+        <v>87062</v>
       </c>
       <c r="Q47">
-        <v>46134</v>
+        <v>87062</v>
       </c>
       <c r="R47" s="1">
-        <v>1.4583333333333334E-3</v>
+        <v>2.2337962962962962E-3</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B48">
         <v>100</v>
@@ -8874,7 +10330,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>161</v>
+        <v>305</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -8883,36 +10339,36 @@
         <v>20</v>
       </c>
       <c r="J48">
-        <v>-1875.6391554812008</v>
+        <v>-5601.3752998833024</v>
       </c>
       <c r="K48">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L48" t="s">
         <v>21</v>
       </c>
       <c r="M48">
-        <v>161</v>
+        <v>305</v>
       </c>
       <c r="N48">
-        <v>161</v>
+        <v>305</v>
       </c>
       <c r="O48">
         <v>0</v>
       </c>
       <c r="P48">
-        <v>28405</v>
+        <v>85524</v>
       </c>
       <c r="Q48">
-        <v>28405</v>
+        <v>85524</v>
       </c>
       <c r="R48" s="1">
-        <v>9.1435185185185185E-4</v>
+        <v>2.3148148148148147E-3</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B49">
         <v>100</v>
@@ -8930,7 +10386,7 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>205</v>
+        <v>309</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -8939,36 +10395,36 @@
         <v>20</v>
       </c>
       <c r="J49">
-        <v>-1877.7194518025144</v>
+        <v>-6497.6808058318993</v>
       </c>
       <c r="K49">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L49" t="s">
         <v>21</v>
       </c>
       <c r="M49">
-        <v>205</v>
+        <v>309</v>
       </c>
       <c r="N49">
-        <v>205</v>
+        <v>309</v>
       </c>
       <c r="O49">
         <v>0</v>
       </c>
       <c r="P49">
-        <v>34921</v>
+        <v>99763</v>
       </c>
       <c r="Q49">
-        <v>34921</v>
+        <v>99763</v>
       </c>
       <c r="R49" s="1">
-        <v>1.7939814814814815E-3</v>
+        <v>2.4189814814814816E-3</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B50">
         <v>100</v>
@@ -8986,7 +10442,7 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>75</v>
+        <v>340</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -8995,36 +10451,36 @@
         <v>20</v>
       </c>
       <c r="J50">
-        <v>-911.22656639553634</v>
+        <v>-4598.7146838560748</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L50" t="s">
         <v>21</v>
       </c>
       <c r="M50">
-        <v>75</v>
+        <v>340</v>
       </c>
       <c r="N50">
-        <v>75</v>
+        <v>340</v>
       </c>
       <c r="O50">
         <v>0</v>
       </c>
       <c r="P50">
-        <v>18196</v>
+        <v>70524</v>
       </c>
       <c r="Q50">
-        <v>18196</v>
+        <v>70524</v>
       </c>
       <c r="R50" s="1">
-        <v>1.7361111111111112E-4</v>
+        <v>4.31712962962963E-3</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B51">
         <v>100</v>
@@ -9042,7 +10498,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>565</v>
+        <v>347</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -9051,36 +10507,36 @@
         <v>20</v>
       </c>
       <c r="J51">
-        <v>-5464.804113587551</v>
+        <v>-8341.8231502604522</v>
       </c>
       <c r="K51">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L51" t="s">
         <v>21</v>
       </c>
       <c r="M51">
-        <v>565</v>
+        <v>347</v>
       </c>
       <c r="N51">
-        <v>565</v>
+        <v>347</v>
       </c>
       <c r="O51">
         <v>0</v>
       </c>
       <c r="P51">
-        <v>106713</v>
+        <v>105397</v>
       </c>
       <c r="Q51">
-        <v>106713</v>
+        <v>105397</v>
       </c>
       <c r="R51" s="1">
-        <v>1.7361111111111112E-2</v>
+        <v>2.8587962962962963E-3</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B52">
         <v>100</v>
@@ -9098,7 +10554,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>251</v>
+        <v>357</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -9107,36 +10563,36 @@
         <v>20</v>
       </c>
       <c r="J52">
-        <v>-3578.8318897373438</v>
+        <v>-4534.480042838667</v>
       </c>
       <c r="K52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L52" t="s">
         <v>21</v>
       </c>
       <c r="M52">
-        <v>251</v>
+        <v>357</v>
       </c>
       <c r="N52">
-        <v>251</v>
+        <v>357</v>
       </c>
       <c r="O52">
         <v>0</v>
       </c>
       <c r="P52">
-        <v>54241</v>
+        <v>83349</v>
       </c>
       <c r="Q52">
-        <v>54241</v>
+        <v>83349</v>
       </c>
       <c r="R52" s="1">
-        <v>2.0486111111111113E-3</v>
+        <v>5.0810185185185186E-3</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B53">
         <v>100</v>
@@ -9154,7 +10610,7 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>25</v>
+        <v>360</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -9163,36 +10619,36 @@
         <v>20</v>
       </c>
       <c r="J53">
-        <v>-931.51751441542706</v>
+        <v>-4471.0601521554308</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L53" t="s">
         <v>21</v>
       </c>
       <c r="M53">
-        <v>25</v>
+        <v>360</v>
       </c>
       <c r="N53">
-        <v>25</v>
+        <v>360</v>
       </c>
       <c r="O53">
         <v>0</v>
       </c>
       <c r="P53">
-        <v>13566</v>
+        <v>77797</v>
       </c>
       <c r="Q53">
-        <v>13566</v>
+        <v>77797</v>
       </c>
       <c r="R53" s="1">
-        <v>0</v>
+        <v>5.4629629629629629E-3</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>100</v>
@@ -9210,7 +10666,7 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>472</v>
+        <v>361</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -9219,36 +10675,36 @@
         <v>20</v>
       </c>
       <c r="J54">
-        <v>-5518.668627373856</v>
+        <v>-3676.7369592406326</v>
       </c>
       <c r="K54">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L54" t="s">
         <v>21</v>
       </c>
       <c r="M54">
-        <v>472</v>
+        <v>361</v>
       </c>
       <c r="N54">
-        <v>472</v>
+        <v>361</v>
       </c>
       <c r="O54">
         <v>0</v>
       </c>
       <c r="P54">
-        <v>106132</v>
+        <v>91105</v>
       </c>
       <c r="Q54">
-        <v>106132</v>
+        <v>91105</v>
       </c>
       <c r="R54" s="1">
-        <v>9.8958333333333329E-3</v>
+        <v>4.7453703703703703E-3</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B55">
         <v>100</v>
@@ -9266,7 +10722,7 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>296</v>
+        <v>388</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -9275,36 +10731,36 @@
         <v>20</v>
       </c>
       <c r="J55">
-        <v>-4619.0395607109003</v>
+        <v>-3698.5274936600208</v>
       </c>
       <c r="K55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L55" t="s">
         <v>21</v>
       </c>
       <c r="M55">
-        <v>296</v>
+        <v>388</v>
       </c>
       <c r="N55">
-        <v>296</v>
+        <v>388</v>
       </c>
       <c r="O55">
         <v>0</v>
       </c>
       <c r="P55">
-        <v>87062</v>
+        <v>80894</v>
       </c>
       <c r="Q55">
-        <v>87062</v>
+        <v>80894</v>
       </c>
       <c r="R55" s="1">
-        <v>2.2337962962962962E-3</v>
+        <v>6.9675925925925929E-3</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B56">
         <v>100</v>
@@ -9322,7 +10778,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>131</v>
+        <v>404</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -9331,36 +10787,36 @@
         <v>20</v>
       </c>
       <c r="J56">
-        <v>-1812.0397117984292</v>
+        <v>-9236.5008999071706</v>
       </c>
       <c r="K56">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L56" t="s">
         <v>21</v>
       </c>
       <c r="M56">
-        <v>131</v>
+        <v>404</v>
       </c>
       <c r="N56">
-        <v>131</v>
+        <v>404</v>
       </c>
       <c r="O56">
         <v>0</v>
       </c>
       <c r="P56">
-        <v>25192</v>
+        <v>139711</v>
       </c>
       <c r="Q56">
-        <v>25192</v>
+        <v>139711</v>
       </c>
       <c r="R56" s="1">
-        <v>6.3657407407407413E-4</v>
+        <v>3.3796296296296296E-3</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B57">
         <v>100</v>
@@ -9378,7 +10834,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>186</v>
+        <v>472</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -9387,36 +10843,36 @@
         <v>20</v>
       </c>
       <c r="J57">
-        <v>-1870.610005459376</v>
+        <v>-5518.668627373856</v>
       </c>
       <c r="K57">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L57" t="s">
         <v>21</v>
       </c>
       <c r="M57">
-        <v>186</v>
+        <v>472</v>
       </c>
       <c r="N57">
-        <v>186</v>
+        <v>472</v>
       </c>
       <c r="O57">
         <v>0</v>
       </c>
       <c r="P57">
-        <v>42531</v>
+        <v>106132</v>
       </c>
       <c r="Q57">
-        <v>42531</v>
+        <v>106132</v>
       </c>
       <c r="R57" s="1">
-        <v>1.1111111111111111E-3</v>
+        <v>9.8958333333333329E-3</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B58">
         <v>100</v>
@@ -9434,7 +10890,7 @@
         <v>0</v>
       </c>
       <c r="G58">
-        <v>164</v>
+        <v>489</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -9443,36 +10899,36 @@
         <v>20</v>
       </c>
       <c r="J58">
-        <v>-1803.7021737658026</v>
+        <v>-9333.8475253964734</v>
       </c>
       <c r="K58">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L58" t="s">
         <v>21</v>
       </c>
       <c r="M58">
-        <v>164</v>
+        <v>489</v>
       </c>
       <c r="N58">
-        <v>164</v>
+        <v>489</v>
       </c>
       <c r="O58">
         <v>0</v>
       </c>
       <c r="P58">
-        <v>28887</v>
+        <v>157856</v>
       </c>
       <c r="Q58">
-        <v>28887</v>
+        <v>157856</v>
       </c>
       <c r="R58" s="1">
-        <v>1.4699074074074074E-3</v>
+        <v>5.4861111111111109E-3</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="B59">
         <v>100</v>
@@ -9490,7 +10946,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>357</v>
+        <v>498</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -9499,36 +10955,36 @@
         <v>20</v>
       </c>
       <c r="J59">
-        <v>-4534.480042838667</v>
+        <v>-11341.325407331695</v>
       </c>
       <c r="K59">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L59" t="s">
         <v>21</v>
       </c>
       <c r="M59">
-        <v>357</v>
+        <v>498</v>
       </c>
       <c r="N59">
-        <v>357</v>
+        <v>498</v>
       </c>
       <c r="O59">
         <v>0</v>
       </c>
       <c r="P59">
-        <v>83349</v>
+        <v>166216</v>
       </c>
       <c r="Q59">
-        <v>83349</v>
+        <v>166216</v>
       </c>
       <c r="R59" s="1">
-        <v>5.0810185185185186E-3</v>
+        <v>5.5787037037037038E-3</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B60">
         <v>100</v>
@@ -9546,7 +11002,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>388</v>
+        <v>565</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -9555,36 +11011,36 @@
         <v>20</v>
       </c>
       <c r="J60">
-        <v>-3698.5274936600208</v>
+        <v>-5464.804113587551</v>
       </c>
       <c r="K60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L60" t="s">
         <v>21</v>
       </c>
       <c r="M60">
-        <v>388</v>
+        <v>565</v>
       </c>
       <c r="N60">
-        <v>388</v>
+        <v>565</v>
       </c>
       <c r="O60">
         <v>0</v>
       </c>
       <c r="P60">
-        <v>80894</v>
+        <v>106713</v>
       </c>
       <c r="Q60">
-        <v>80894</v>
+        <v>106713</v>
       </c>
       <c r="R60" s="1">
-        <v>6.9675925925925929E-3</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B61">
         <v>100</v>
@@ -9602,7 +11058,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>360</v>
+        <v>616</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -9611,31 +11067,31 @@
         <v>20</v>
       </c>
       <c r="J61">
-        <v>-4471.0601521554308</v>
+        <v>-8329.2999785437587</v>
       </c>
       <c r="K61">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L61" t="s">
         <v>21</v>
       </c>
       <c r="M61">
-        <v>360</v>
+        <v>616</v>
       </c>
       <c r="N61">
-        <v>360</v>
+        <v>616</v>
       </c>
       <c r="O61">
         <v>0</v>
       </c>
       <c r="P61">
-        <v>77797</v>
+        <v>137832</v>
       </c>
       <c r="Q61">
-        <v>77797</v>
+        <v>137832</v>
       </c>
       <c r="R61" s="1">
-        <v>5.4629629629629629E-3</v>
+        <v>1.375E-2</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -9645,7 +11101,7 @@
       </c>
       <c r="J62">
         <f>SUM(Carriers_stats[jSpritScoreSelectedPlan])</f>
-        <v>-192294.19944953761</v>
+        <v>-192294.19944953758</v>
       </c>
       <c r="K62">
         <f>SUM(Carriers_stats[nuOfTours])</f>
@@ -9657,13 +11113,14 @@
       </c>
       <c r="R62" s="1">
         <f>SUM(Carriers_stats[jspritComputationTime])</f>
-        <v>0.12480324074074076</v>
+        <v>0.12480324074074074</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>